<commit_message>
FixedBase Class issues and added Reports and Screenshots
</commit_message>
<xml_diff>
--- a/TestData/Data.xlsx
+++ b/TestData/Data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Search Text</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>c</t>
+  </si>
+  <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>Samsung 138 cm (55 Inches) Super 6 Series 4K UHD LED Smart TV UA55NU6100 (Black) (2019 model)</t>
   </si>
 </sst>
 </file>
@@ -376,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -421,6 +427,14 @@
         <v>8</v>
       </c>
     </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>

</xml_diff>